<commit_message>
chore:add 2-5-1 HW folder
</commit_message>
<xml_diff>
--- a/0.商務軟體分析_專題製作/UML/商品管理與販售平台系統資料規格.xlsx
+++ b/0.商務軟體分析_專題製作/UML/商品管理與販售平台系統資料規格.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\0.Homework\0.商務軟體分析_專題製作\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEBD9BE-A743-4F7D-900B-24C1B05151CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCD0352-1883-4E4E-A5A8-595F9A470A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{C044DA50-0112-404E-A9D3-A86B7E7712CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C044DA50-0112-404E-A9D3-A86B7E7712CE}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="99">
   <si>
     <t xml:space="preserve"> Entity：會員  Table Name : Member</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -414,6 +414,10 @@
   </si>
   <si>
     <t xml:space="preserve"> Entity：會員手機  Table Name : MemberTel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Entity：商場  Table Name : MemberStore</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +550,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -565,14 +569,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEA3CBF-AB68-4CCD-A92A-FF42B1F61844}">
-  <dimension ref="B2:H65"/>
+  <dimension ref="B2:T80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -906,26 +919,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -1048,15 +1070,15 @@
       <c r="H10" s="3"/>
     </row>
     <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1121,7 +1143,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1144,18 +1166,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1178,7 +1200,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
@@ -1199,7 +1221,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>35</v>
       </c>
@@ -1218,7 +1240,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1241,18 +1263,34 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="2:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
@@ -1274,19 +1312,26 @@
       <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="N28" s="2"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>11</v>
@@ -1294,368 +1339,320 @@
       <c r="G29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E30" s="3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="N30" s="2"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="2:20" ht="21" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E31" s="3">
+        <v>5</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="3" t="s">
-        <v>51</v>
+      <c r="G31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="42" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="5">
+      <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="3">
-        <v>400</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="3">
-        <v>2</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="3">
-        <v>2</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3">
+        <v>5</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E45" s="3">
+        <v>40</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="47" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+      <c r="E48" s="5">
         <v>1</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>7</v>
+      <c r="F48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="3">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="E49" s="5">
+        <v>2</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="3"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="50" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>47</v>
+        <v>16</v>
+      </c>
+      <c r="E50" s="3">
+        <v>400</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="4"/>
-      <c r="H50" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="H50" s="3"/>
     </row>
     <row r="51" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>47</v>
+        <v>16</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="G51" s="4"/>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>23</v>
@@ -1666,220 +1663,172 @@
       <c r="F52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="4"/>
+      <c r="G53" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H53" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C54" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="3" t="s">
+    </row>
+    <row r="58" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E54" s="3">
-        <v>200</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="E59" s="3">
         <v>10</v>
       </c>
-      <c r="E55" s="3">
+      <c r="F59" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="62" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="8"/>
+    </row>
+    <row r="63" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G59" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="H63" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="3">
-        <v>12</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="3">
-        <v>5</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="3"/>
     </row>
     <row r="64" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E64" s="3">
+        <v>12</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G64" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="2:8" ht="21" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>47</v>
@@ -1887,21 +1836,284 @@
       <c r="F65" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="3"/>
+      <c r="G65" s="4"/>
       <c r="H65" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="3" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="69" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="3">
+        <v>200</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="3">
+        <v>5</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="8"/>
+    </row>
+    <row r="74" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="3">
+        <v>12</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="3">
+        <v>5</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" s="4"/>
+      <c r="H77" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G78" s="4"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="N26:T26"/>
+    <mergeCell ref="B27:H27"/>
     <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B58:H58"/>
+    <mergeCell ref="B73:H73"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B62:H62"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>